<commit_message>
Add new Image, create tranformation method and GeneretionLinesOfLimits Method
</commit_message>
<xml_diff>
--- a/TrabalhoCP2/Resources/Calculator/HResolve.xlsx
+++ b/TrabalhoCP2/Resources/Calculator/HResolve.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -105,8 +105,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="172" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -210,7 +213,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -236,19 +239,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="23">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -260,6 +261,17 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink seguido" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink seguido" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink seguido" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink seguido" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink seguido" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink seguido" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink seguido" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink seguido" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink seguido" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink seguido" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink seguido" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -588,24 +600,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M51" sqref="M51"/>
+    <sheetView tabSelected="1" topLeftCell="G31" workbookViewId="0">
+      <selection activeCell="L45" sqref="J43:L45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="3"/>
+    <col min="1" max="2" width="10.796875" style="3"/>
     <col min="3" max="3" width="13" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.796875" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="10.83203125" style="3"/>
+    <col min="6" max="7" width="12.19921875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.19921875" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.19921875" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="10.796875" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:17">
@@ -613,10 +627,10 @@
         <v>17</v>
       </c>
       <c r="C2" s="3">
-        <v>168</v>
+        <v>417</v>
       </c>
       <c r="D2" s="3">
-        <v>106</v>
+        <v>39</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>21</v>
@@ -633,16 +647,16 @@
         <v>18</v>
       </c>
       <c r="C3" s="3">
-        <v>369</v>
+        <v>861</v>
       </c>
       <c r="D3" s="3">
-        <v>80</v>
+        <v>39</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G3" s="3">
-        <v>878</v>
+        <v>1920</v>
       </c>
       <c r="H3" s="3">
         <v>0</v>
@@ -653,19 +667,19 @@
         <v>19</v>
       </c>
       <c r="C4" s="3">
-        <v>373</v>
+        <v>771</v>
       </c>
       <c r="D4" s="3">
-        <v>309</v>
+        <v>130</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>23</v>
       </c>
       <c r="G4" s="3">
-        <v>878</v>
+        <v>1920</v>
       </c>
       <c r="H4" s="3">
-        <v>878</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -673,10 +687,10 @@
         <v>20</v>
       </c>
       <c r="C5" s="3">
-        <v>158</v>
+        <v>441</v>
       </c>
       <c r="D5" s="3">
-        <v>313</v>
+        <v>130</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>24</v>
@@ -685,7 +699,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="3">
-        <v>878</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="8" spans="1:17" s="1" customFormat="1">
@@ -732,11 +746,11 @@
       </c>
       <c r="C9" s="4">
         <f>C2</f>
-        <v>168</v>
+        <v>417</v>
       </c>
       <c r="D9" s="3">
         <f>D2</f>
-        <v>106</v>
+        <v>39</v>
       </c>
       <c r="E9" s="3">
         <v>1</v>
@@ -787,11 +801,11 @@
       </c>
       <c r="F10" s="7">
         <f>C2</f>
-        <v>168</v>
+        <v>417</v>
       </c>
       <c r="G10" s="7">
         <f>D2</f>
-        <v>106</v>
+        <v>39</v>
       </c>
       <c r="H10" s="7">
         <v>1</v>
@@ -842,11 +856,11 @@
       </c>
       <c r="I11" s="7">
         <f>C2</f>
-        <v>168</v>
+        <v>417</v>
       </c>
       <c r="J11" s="7">
         <f>D2</f>
-        <v>106</v>
+        <v>39</v>
       </c>
       <c r="K11" s="7">
         <v>1</v>
@@ -870,11 +884,11 @@
       </c>
       <c r="C12" s="4">
         <f>C3</f>
-        <v>369</v>
+        <v>861</v>
       </c>
       <c r="D12" s="7">
         <f>D3</f>
-        <v>80</v>
+        <v>39</v>
       </c>
       <c r="E12" s="7">
         <v>1</v>
@@ -902,7 +916,7 @@
       </c>
       <c r="M12" s="3">
         <f>-G3</f>
-        <v>-878</v>
+        <v>-1920</v>
       </c>
       <c r="N12" s="5">
         <v>0</v>
@@ -926,11 +940,11 @@
       </c>
       <c r="F13" s="7">
         <f>C3</f>
-        <v>369</v>
+        <v>861</v>
       </c>
       <c r="G13" s="7">
         <f>D3</f>
-        <v>80</v>
+        <v>39</v>
       </c>
       <c r="H13" s="7">
         <v>1</v>
@@ -981,11 +995,11 @@
       </c>
       <c r="I14" s="7">
         <f>C3</f>
-        <v>369</v>
+        <v>861</v>
       </c>
       <c r="J14" s="7">
         <f>D3</f>
-        <v>80</v>
+        <v>39</v>
       </c>
       <c r="K14" s="7">
         <v>1</v>
@@ -1012,11 +1026,11 @@
       </c>
       <c r="C15" s="4">
         <f>C4</f>
-        <v>373</v>
+        <v>771</v>
       </c>
       <c r="D15" s="7">
         <f>D4</f>
-        <v>309</v>
+        <v>130</v>
       </c>
       <c r="E15" s="7">
         <v>1</v>
@@ -1047,7 +1061,7 @@
       </c>
       <c r="N15" s="5">
         <f>-G4</f>
-        <v>-878</v>
+        <v>-1920</v>
       </c>
       <c r="P15" s="3" t="s">
         <v>13</v>
@@ -1071,11 +1085,11 @@
       </c>
       <c r="F16" s="7">
         <f>C4</f>
-        <v>373</v>
+        <v>771</v>
       </c>
       <c r="G16" s="7">
         <f>D4</f>
-        <v>309</v>
+        <v>130</v>
       </c>
       <c r="H16" s="7">
         <v>1</v>
@@ -1097,7 +1111,7 @@
       </c>
       <c r="N16" s="5">
         <f>-H4</f>
-        <v>-878</v>
+        <v>-1200</v>
       </c>
       <c r="Q16" s="6">
         <v>0</v>
@@ -1127,11 +1141,11 @@
       </c>
       <c r="I17" s="7">
         <f>C4</f>
-        <v>373</v>
+        <v>771</v>
       </c>
       <c r="J17" s="7">
         <f>D4</f>
-        <v>309</v>
+        <v>130</v>
       </c>
       <c r="K17" s="7">
         <v>1</v>
@@ -1155,11 +1169,11 @@
       </c>
       <c r="C18" s="4">
         <f>C5</f>
-        <v>158</v>
+        <v>441</v>
       </c>
       <c r="D18" s="7">
         <f>D5</f>
-        <v>313</v>
+        <v>130</v>
       </c>
       <c r="E18" s="7">
         <v>1</v>
@@ -1210,11 +1224,11 @@
       </c>
       <c r="F19" s="7">
         <f>C5</f>
-        <v>158</v>
+        <v>441</v>
       </c>
       <c r="G19" s="7">
         <f>D5</f>
-        <v>313</v>
+        <v>130</v>
       </c>
       <c r="H19" s="7">
         <v>1</v>
@@ -1239,7 +1253,7 @@
       </c>
       <c r="Q19" s="6">
         <f>H5</f>
-        <v>878</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -1266,11 +1280,11 @@
       </c>
       <c r="I20" s="7">
         <f>C5</f>
-        <v>158</v>
+        <v>441</v>
       </c>
       <c r="J20" s="7">
         <f>D5</f>
-        <v>313</v>
+        <v>130</v>
       </c>
       <c r="K20" s="7">
         <v>1</v>
@@ -1314,10 +1328,10 @@
       </c>
       <c r="C24" s="4">
         <f t="array" ref="C24:N35">MINVERSE(C9:N20)</f>
-        <v>-8.9958394242664036E-5</v>
+        <v>2.5789152720677272E-19</v>
       </c>
       <c r="D24" s="7">
-        <v>-5.5452751172575671E-3</v>
+        <v>-3.6036036036036041E-3</v>
       </c>
       <c r="E24" s="7">
         <v>0</v>
@@ -1326,32 +1340,32 @@
         <v>0</v>
       </c>
       <c r="G24" s="7">
-        <v>5.0064091711611485E-3</v>
+        <v>3.6036036036036041E-3</v>
       </c>
       <c r="H24" s="7">
         <v>0</v>
       </c>
       <c r="I24" s="7">
-        <v>4.6553469020577986E-3</v>
+        <v>3.0303030303030307E-3</v>
       </c>
       <c r="J24" s="7">
-        <v>-4.6553469020577994E-3</v>
+        <v>-4.8484848484848502E-3</v>
       </c>
       <c r="K24" s="7">
         <v>0</v>
       </c>
       <c r="L24" s="7">
-        <v>-4.5653885078151355E-3</v>
+        <v>-3.0303030303030307E-3</v>
       </c>
       <c r="M24" s="7">
-        <v>5.194212848154218E-3</v>
+        <v>4.8484848484848502E-3</v>
       </c>
       <c r="N24" s="5">
         <v>0</v>
       </c>
       <c r="Q24" s="6">
         <f t="array" ref="Q24:Q35">MMULT(C24:N35, Q9:Q20)</f>
-        <v>4.5605188806794033</v>
+        <v>5.8181818181818201</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -1359,10 +1373,10 @@
         <v>2</v>
       </c>
       <c r="C25" s="4">
-        <v>-4.8352636905431229E-3</v>
+        <v>-1.0989010989010988E-2</v>
       </c>
       <c r="D25" s="7">
-        <v>-2.6788768682403825E-4</v>
+        <v>9.5040095040095044E-4</v>
       </c>
       <c r="E25" s="7">
         <v>0</v>
@@ -1371,31 +1385,31 @@
         <v>0</v>
       </c>
       <c r="G25" s="7">
-        <v>2.41855515515032E-4</v>
+        <v>-9.5040095040095044E-4</v>
       </c>
       <c r="H25" s="7">
         <v>0</v>
       </c>
       <c r="I25" s="7">
-        <v>2.248959856066574E-4</v>
+        <v>-7.992007992007992E-4</v>
       </c>
       <c r="J25" s="7">
-        <v>-2.2489598560665789E-4</v>
+        <v>1.2787212787212805E-3</v>
       </c>
       <c r="K25" s="7">
         <v>0</v>
       </c>
       <c r="L25" s="7">
-        <v>4.6103677049364666E-3</v>
+        <v>1.1788211788211787E-2</v>
       </c>
       <c r="M25" s="7">
-        <v>2.5092815691566219E-4</v>
+        <v>-1.2787212787212805E-3</v>
       </c>
       <c r="N25" s="5">
         <v>0</v>
       </c>
       <c r="Q25" s="6">
-        <v>0.22031492177195142</v>
+        <v>-1.5344655344655365</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -1403,10 +1417,10 @@
         <v>3</v>
       </c>
       <c r="C26" s="4">
-        <v>1.5276509614303386</v>
+        <v>1.4285714285714284</v>
       </c>
       <c r="D26" s="7">
-        <v>0.96000231450261952</v>
+        <v>1.4656370656370659</v>
       </c>
       <c r="E26" s="7">
         <v>0</v>
@@ -1415,31 +1429,31 @@
         <v>0</v>
       </c>
       <c r="G26" s="7">
-        <v>-0.86671342539966634</v>
+        <v>-1.4656370656370659</v>
       </c>
       <c r="H26" s="7">
         <v>0</v>
       </c>
       <c r="I26" s="7">
-        <v>-0.80593725402001593</v>
+        <v>-1.2324675324675327</v>
       </c>
       <c r="J26" s="7">
-        <v>0.80593725402001637</v>
+        <v>1.9719480519480523</v>
       </c>
       <c r="K26" s="7">
         <v>0</v>
       </c>
       <c r="L26" s="7">
-        <v>0.27828629258967752</v>
+        <v>0.803896103896104</v>
       </c>
       <c r="M26" s="7">
-        <v>-0.89922614312296911</v>
+        <v>-1.9719480519480523</v>
       </c>
       <c r="N26" s="5">
         <v>0</v>
       </c>
       <c r="Q26" s="6">
-        <v>-789.52055366196691</v>
+        <v>-2366.337662337663</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -1450,7 +1464,7 @@
         <v>0</v>
       </c>
       <c r="D27" s="7">
-        <v>-5.635233511500231E-3</v>
+        <v>-2.2522522522522527E-3</v>
       </c>
       <c r="E27" s="7">
         <v>0</v>
@@ -1459,7 +1473,7 @@
         <v>0</v>
       </c>
       <c r="G27" s="7">
-        <v>5.0064091711611485E-3</v>
+        <v>2.2522522522522522E-3</v>
       </c>
       <c r="H27" s="7">
         <v>0</v>
@@ -1468,7 +1482,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="7">
-        <v>-8.9294077047599723E-19</v>
+        <v>0</v>
       </c>
       <c r="K27" s="7">
         <v>0</v>
@@ -1477,13 +1491,13 @@
         <v>0</v>
       </c>
       <c r="M27" s="7">
-        <v>6.2882434033908281E-4</v>
+        <v>0</v>
       </c>
       <c r="N27" s="5">
         <v>0</v>
       </c>
       <c r="Q27" s="6">
-        <v>0.55210777081771467</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -1494,7 +1508,7 @@
         <v>0</v>
       </c>
       <c r="D28" s="7">
-        <v>-5.103151377367162E-3</v>
+        <v>-1.0395010395010394E-2</v>
       </c>
       <c r="E28" s="7">
         <v>0</v>
@@ -1503,7 +1517,7 @@
         <v>0</v>
       </c>
       <c r="G28" s="7">
-        <v>2.41855515515032E-4</v>
+        <v>-5.9400059400059417E-4</v>
       </c>
       <c r="H28" s="7">
         <v>0</v>
@@ -1512,7 +1526,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="7">
-        <v>-4.9193189459044605E-19</v>
+        <v>0</v>
       </c>
       <c r="K28" s="7">
         <v>0</v>
@@ -1521,13 +1535,13 @@
         <v>0</v>
       </c>
       <c r="M28" s="7">
-        <v>4.8612958618521286E-3</v>
+        <v>1.0989010989010988E-2</v>
       </c>
       <c r="N28" s="5">
         <v>0</v>
       </c>
       <c r="Q28" s="6">
-        <v>4.2682177667061687</v>
+        <v>13.186813186813186</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -1538,7 +1552,7 @@
         <v>0</v>
       </c>
       <c r="D29" s="7">
-        <v>2.4876532759329582</v>
+        <v>2.3445945945945947</v>
       </c>
       <c r="E29" s="7">
         <v>0</v>
@@ -1547,7 +1561,7 @@
         <v>0</v>
       </c>
       <c r="G29" s="7">
-        <v>-0.86671342539966634</v>
+        <v>-0.91602316602316602</v>
       </c>
       <c r="H29" s="7">
         <v>0</v>
@@ -1556,7 +1570,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="7">
-        <v>3.7952400737434902E-16</v>
+        <v>0</v>
       </c>
       <c r="K29" s="7">
         <v>0</v>
@@ -1565,13 +1579,13 @@
         <v>0</v>
       </c>
       <c r="M29" s="7">
-        <v>-0.62093985053329159</v>
+        <v>-0.42857142857142855</v>
       </c>
       <c r="N29" s="5">
         <v>0</v>
       </c>
       <c r="Q29" s="6">
-        <v>-545.18518876822998</v>
+        <v>-514.28571428571422</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -1582,46 +1596,46 @@
         <v>14</v>
       </c>
       <c r="C30" s="4">
-        <v>-1.0245830779346619E-7</v>
+        <v>0</v>
       </c>
       <c r="D30" s="7">
-        <v>-6.3158030948263884E-6</v>
+        <v>-1.8768768768768768E-6</v>
       </c>
       <c r="E30" s="7">
         <v>0</v>
       </c>
       <c r="F30" s="7">
-        <v>9.2501850846408461E-8</v>
+        <v>0</v>
       </c>
       <c r="G30" s="7">
-        <v>5.7020605594090548E-6</v>
+        <v>1.8768768768768768E-6</v>
       </c>
       <c r="H30" s="7">
-        <v>-8.121662504314695E-5</v>
+        <v>2.5789152720677272E-19</v>
       </c>
       <c r="I30" s="7">
-        <v>-8.6015383491431489E-8</v>
+        <v>-1.2592359726893199E-22</v>
       </c>
       <c r="J30" s="7">
-        <v>-5.3022174283118444E-6</v>
+        <v>-2.5252525252525262E-6</v>
       </c>
       <c r="K30" s="7">
-        <v>4.7308684087632741E-3</v>
+        <v>3.0303030303030307E-3</v>
       </c>
       <c r="L30" s="7">
-        <v>9.5971840438488055E-8</v>
+        <v>1.2592359726893199E-22</v>
       </c>
       <c r="M30" s="7">
-        <v>5.915959963729178E-6</v>
+        <v>2.5252525252525262E-6</v>
       </c>
       <c r="N30" s="5">
-        <v>-4.6496517837201282E-3</v>
+        <v>-3.0303030303030303E-3</v>
       </c>
       <c r="P30" s="3" t="s">
         <v>15</v>
       </c>
       <c r="Q30" s="6">
-        <v>5.4456106443408984E-4</v>
+        <v>1.3010426069826053E-18</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -1629,43 +1643,43 @@
         <v>8</v>
       </c>
       <c r="C31" s="4">
-        <v>-5.5071340438987741E-6</v>
+        <v>-5.7234432234432226E-6</v>
       </c>
       <c r="D31" s="7">
-        <v>-3.0511126061963322E-7</v>
+        <v>4.950004950004949E-7</v>
       </c>
       <c r="E31" s="7">
         <v>0</v>
       </c>
       <c r="F31" s="7">
-        <v>4.9719744829944357E-6</v>
+        <v>5.7234432234432226E-6</v>
       </c>
       <c r="G31" s="7">
-        <v>2.7546186277338485E-7</v>
+        <v>-4.950004950004949E-7</v>
       </c>
       <c r="H31" s="7">
-        <v>-4.3653935960691155E-3</v>
+        <v>-1.0989010989010988E-2</v>
       </c>
       <c r="I31" s="7">
-        <v>-4.6233268626643632E-6</v>
+        <v>-7.7006327006327023E-6</v>
       </c>
       <c r="J31" s="7">
-        <v>-2.561457694836649E-7</v>
+        <v>6.6600066600066676E-7</v>
       </c>
       <c r="K31" s="7">
-        <v>4.2841769710259695E-3</v>
+        <v>1.3986013986013986E-2</v>
       </c>
       <c r="L31" s="7">
-        <v>5.1584864235687015E-6</v>
+        <v>7.7006327006327023E-6</v>
       </c>
       <c r="M31" s="7">
-        <v>2.8579516732991226E-7</v>
+        <v>-6.6600066600066676E-7</v>
       </c>
       <c r="N31" s="5">
-        <v>8.1216625043146394E-5</v>
+        <v>-2.9970029970029966E-3</v>
       </c>
       <c r="Q31" s="6">
-        <v>3.3214478195880937E-4</v>
+        <v>-3.7962037962037966E-3</v>
       </c>
     </row>
     <row r="32" spans="1:17">
@@ -1673,43 +1687,43 @@
         <v>9</v>
       </c>
       <c r="C32" s="4">
-        <v>1.739921368371684E-3</v>
+        <v>7.4404761904761901E-4</v>
       </c>
       <c r="D32" s="7">
-        <v>1.0933967135565146E-3</v>
+        <v>7.6335263835263835E-4</v>
       </c>
       <c r="E32" s="7">
         <v>0</v>
       </c>
       <c r="F32" s="7">
-        <v>-1.5708433056109911E-3</v>
+        <v>-7.4404761904761901E-4</v>
       </c>
       <c r="G32" s="7">
-        <v>-9.8714513143470018E-4</v>
+        <v>-7.6335263835263835E-4</v>
       </c>
       <c r="H32" s="7">
-        <v>1.3792004223264505</v>
+        <v>1.4285714285714284</v>
       </c>
       <c r="I32" s="7">
-        <v>1.4606917386055921E-3</v>
+        <v>1.0010822510822513E-3</v>
       </c>
       <c r="J32" s="7">
-        <v>9.1792397952165873E-4</v>
+        <v>1.0270562770562772E-3</v>
       </c>
       <c r="K32" s="7">
-        <v>-2.0884246005157259</v>
+        <v>-3.1545454545454548</v>
       </c>
       <c r="L32" s="7">
-        <v>-1.6297698013662848E-3</v>
+        <v>-1.0010822510822513E-3</v>
       </c>
       <c r="M32" s="7">
-        <v>-1.0241755616434728E-3</v>
+        <v>-1.0270562770562772E-3</v>
       </c>
       <c r="N32" s="5">
-        <v>1.7092241781892756</v>
+        <v>2.7259740259740259</v>
       </c>
       <c r="Q32" s="6">
-        <v>0.80999803506630652</v>
+        <v>1.4935064935064934</v>
       </c>
     </row>
     <row r="33" spans="1:17">
@@ -1717,43 +1731,43 @@
         <v>10</v>
       </c>
       <c r="C33" s="4">
-        <v>1.1389521640091116E-3</v>
+        <v>5.2083333333333333E-4</v>
       </c>
       <c r="D33" s="7">
-        <v>2.1684043449710089E-19</v>
+        <v>0</v>
       </c>
       <c r="E33" s="7">
         <v>-1</v>
       </c>
       <c r="F33" s="7">
-        <v>-1.0282736994713841E-3</v>
+        <v>-5.2083333333333333E-4</v>
       </c>
       <c r="G33" s="7">
-        <v>-2.1684043449710089E-19</v>
+        <v>0</v>
       </c>
       <c r="H33" s="7">
-        <v>0.90282430813587533</v>
+        <v>1</v>
       </c>
       <c r="I33" s="7">
-        <v>9.5616850673660892E-4</v>
+        <v>7.0075757575757582E-4</v>
       </c>
       <c r="J33" s="7">
-        <v>3.2526065174565133E-19</v>
+        <v>0</v>
       </c>
       <c r="K33" s="7">
-        <v>-0.83951594891474279</v>
+        <v>-1.3454545454545455</v>
       </c>
       <c r="L33" s="7">
-        <v>-1.0668469712743363E-3</v>
+        <v>-7.0075757575757582E-4</v>
       </c>
       <c r="M33" s="7">
-        <v>-2.1684043449710089E-19</v>
+        <v>0</v>
       </c>
       <c r="N33" s="5">
-        <v>0.93669164077886735</v>
+        <v>1.3454545454545455</v>
       </c>
       <c r="Q33" s="6">
-        <v>0.93669164077886713</v>
+        <v>1.3454545454545455</v>
       </c>
     </row>
     <row r="34" spans="1:17">
@@ -1761,43 +1775,43 @@
         <v>11</v>
       </c>
       <c r="C34" s="4">
-        <v>1.2615435292839931E-3</v>
+        <v>5.2083333333333333E-4</v>
       </c>
       <c r="D34" s="7">
-        <v>-1.2615435292839931E-3</v>
+        <v>-8.3333333333333328E-4</v>
       </c>
       <c r="E34" s="7">
         <v>0</v>
       </c>
       <c r="F34" s="7">
-        <v>-1.1389521640091116E-3</v>
+        <v>-5.2083333333333333E-4</v>
       </c>
       <c r="G34" s="7">
-        <v>1.1389521640091116E-3</v>
+        <v>8.3333333333333328E-4</v>
       </c>
       <c r="H34" s="7">
         <v>0</v>
       </c>
       <c r="I34" s="7">
-        <v>1.059085913084105E-3</v>
+        <v>7.0075757575757582E-4</v>
       </c>
       <c r="J34" s="7">
-        <v>-1.059085913084105E-3</v>
+        <v>-1.1212121212121214E-3</v>
       </c>
       <c r="K34" s="7">
         <v>0</v>
       </c>
       <c r="L34" s="7">
-        <v>-1.1816772783589866E-3</v>
+        <v>-7.0075757575757582E-4</v>
       </c>
       <c r="M34" s="7">
-        <v>1.1816772783589866E-3</v>
+        <v>1.1212121212121214E-3</v>
       </c>
       <c r="N34" s="5">
         <v>0</v>
       </c>
       <c r="Q34" s="6">
-        <v>1.0375126503991903</v>
+        <v>1.3454545454545457</v>
       </c>
     </row>
     <row r="35" spans="1:17">
@@ -1808,7 +1822,7 @@
         <v>0</v>
       </c>
       <c r="D35" s="7">
-        <v>-1.3566772203451947E-3</v>
+        <v>-6.1936936936936933E-4</v>
       </c>
       <c r="E35" s="7">
         <v>0</v>
@@ -1817,7 +1831,7 @@
         <v>0</v>
       </c>
       <c r="G35" s="7">
-        <v>1.2248411728218529E-3</v>
+        <v>6.1936936936936933E-4</v>
       </c>
       <c r="H35" s="7">
         <v>0</v>
@@ -1826,7 +1840,7 @@
         <v>0</v>
       </c>
       <c r="J35" s="7">
-        <v>-1.1389521640091118E-3</v>
+        <v>-8.3333333333333339E-4</v>
       </c>
       <c r="K35" s="7">
         <v>0</v>
@@ -1835,13 +1849,13 @@
         <v>0</v>
       </c>
       <c r="M35" s="7">
-        <v>1.2707882115324534E-3</v>
+        <v>8.3333333333333339E-4</v>
       </c>
       <c r="N35" s="5">
         <v>0</v>
       </c>
       <c r="Q35" s="6">
-        <v>1.115752049725494</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:17">
@@ -1853,7 +1867,7 @@
       </c>
       <c r="E40" s="3">
         <f>Q24</f>
-        <v>4.5605188806794033</v>
+        <v>5.8181818181818201</v>
       </c>
     </row>
     <row r="41" spans="1:17">
@@ -1862,7 +1876,7 @@
       </c>
       <c r="E41" s="3">
         <f t="shared" ref="E41:E51" si="0">Q25</f>
-        <v>0.22031492177195142</v>
+        <v>-1.5344655344655365</v>
       </c>
     </row>
     <row r="42" spans="1:17">
@@ -1871,7 +1885,7 @@
       </c>
       <c r="E42" s="3">
         <f t="shared" si="0"/>
-        <v>-789.52055366196691</v>
+        <v>-2366.337662337663</v>
       </c>
     </row>
     <row r="43" spans="1:17">
@@ -1880,19 +1894,19 @@
       </c>
       <c r="E43" s="3">
         <f t="shared" si="0"/>
-        <v>0.55210777081771467</v>
-      </c>
-      <c r="J43" s="4">
+        <v>0</v>
+      </c>
+      <c r="J43" s="9">
         <f>E40</f>
-        <v>4.5605188806794033</v>
-      </c>
-      <c r="K43" s="7">
+        <v>5.8181818181818201</v>
+      </c>
+      <c r="K43" s="10">
         <f>E41</f>
-        <v>0.22031492177195142</v>
-      </c>
-      <c r="L43" s="5">
+        <v>-1.5344655344655365</v>
+      </c>
+      <c r="L43" s="11">
         <f>E42</f>
-        <v>-789.52055366196691</v>
+        <v>-2366.337662337663</v>
       </c>
     </row>
     <row r="44" spans="1:17">
@@ -1901,22 +1915,22 @@
       </c>
       <c r="E44" s="3">
         <f t="shared" si="0"/>
-        <v>4.2682177667061687</v>
+        <v>13.186813186813186</v>
       </c>
       <c r="I44" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J44" s="4">
+      <c r="J44" s="9">
         <f>E43</f>
-        <v>0.55210777081771467</v>
-      </c>
-      <c r="K44" s="7">
+        <v>0</v>
+      </c>
+      <c r="K44" s="10">
         <f>E44</f>
-        <v>4.2682177667061687</v>
-      </c>
-      <c r="L44" s="5">
+        <v>13.186813186813186</v>
+      </c>
+      <c r="L44" s="11">
         <f>E45</f>
-        <v>-545.18518876822998</v>
+        <v>-514.28571428571422</v>
       </c>
     </row>
     <row r="45" spans="1:17">
@@ -1925,19 +1939,19 @@
       </c>
       <c r="E45" s="3">
         <f t="shared" si="0"/>
-        <v>-545.18518876822998</v>
-      </c>
-      <c r="J45" s="4">
+        <v>-514.28571428571422</v>
+      </c>
+      <c r="J45" s="9">
         <f>E46</f>
-        <v>5.4456106443408984E-4</v>
-      </c>
-      <c r="K45" s="7">
+        <v>1.3010426069826053E-18</v>
+      </c>
+      <c r="K45" s="10">
         <f>E47</f>
-        <v>3.3214478195880937E-4</v>
-      </c>
-      <c r="L45" s="5">
+        <v>-3.7962037962037966E-3</v>
+      </c>
+      <c r="L45" s="11">
         <f>E48</f>
-        <v>0.80999803506630652</v>
+        <v>1.4935064935064934</v>
       </c>
     </row>
     <row r="46" spans="1:17">
@@ -1946,7 +1960,7 @@
       </c>
       <c r="E46" s="3">
         <f t="shared" si="0"/>
-        <v>5.4456106443408984E-4</v>
+        <v>1.3010426069826053E-18</v>
       </c>
     </row>
     <row r="47" spans="1:17">
@@ -1955,7 +1969,7 @@
       </c>
       <c r="E47" s="3">
         <f t="shared" si="0"/>
-        <v>3.3214478195880937E-4</v>
+        <v>-3.7962037962037966E-3</v>
       </c>
     </row>
     <row r="48" spans="1:17">
@@ -1964,14 +1978,14 @@
       </c>
       <c r="E48" s="3">
         <f t="shared" si="0"/>
-        <v>0.80999803506630652</v>
+        <v>1.4935064935064934</v>
       </c>
       <c r="I48" s="3" t="s">
         <v>26</v>
       </c>
       <c r="J48" s="6">
         <f>E49</f>
-        <v>0.93669164077886713</v>
+        <v>1.3454545454545455</v>
       </c>
     </row>
     <row r="49" spans="4:10">
@@ -1980,11 +1994,11 @@
       </c>
       <c r="E49" s="3">
         <f t="shared" si="0"/>
-        <v>0.93669164077886713</v>
+        <v>1.3454545454545455</v>
       </c>
       <c r="J49" s="6">
         <f>E50</f>
-        <v>1.0375126503991903</v>
+        <v>1.3454545454545457</v>
       </c>
     </row>
     <row r="50" spans="4:10">
@@ -1993,11 +2007,11 @@
       </c>
       <c r="E50" s="3">
         <f t="shared" si="0"/>
-        <v>1.0375126503991903</v>
+        <v>1.3454545454545457</v>
       </c>
       <c r="J50" s="6">
         <f>E51</f>
-        <v>1.115752049725494</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="4:10">
@@ -2006,7 +2020,7 @@
       </c>
       <c r="E51" s="3">
         <f t="shared" si="0"/>
-        <v>1.115752049725494</v>
+        <v>1</v>
       </c>
       <c r="J51" s="6">
         <f>E52</f>

</xml_diff>

<commit_message>
Teste1 for program execution
</commit_message>
<xml_diff>
--- a/TrabalhoCP2/Resources/Calculator/HResolve.xlsx
+++ b/TrabalhoCP2/Resources/Calculator/HResolve.xlsx
@@ -107,7 +107,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -239,13 +239,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -603,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G31" workbookViewId="0">
-      <selection activeCell="L45" sqref="J43:L45"/>
+    <sheetView tabSelected="1" topLeftCell="G27" workbookViewId="0">
+      <selection activeCell="N47" sqref="N47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
@@ -627,10 +627,10 @@
         <v>17</v>
       </c>
       <c r="C2" s="3">
-        <v>417</v>
+        <v>57</v>
       </c>
       <c r="D2" s="3">
-        <v>39</v>
+        <v>211</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>21</v>
@@ -647,16 +647,16 @@
         <v>18</v>
       </c>
       <c r="C3" s="3">
-        <v>861</v>
+        <v>231</v>
       </c>
       <c r="D3" s="3">
-        <v>39</v>
+        <v>211</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G3" s="3">
-        <v>1920</v>
+        <v>1024</v>
       </c>
       <c r="H3" s="3">
         <v>0</v>
@@ -667,19 +667,19 @@
         <v>19</v>
       </c>
       <c r="C4" s="3">
-        <v>771</v>
+        <v>231</v>
       </c>
       <c r="D4" s="3">
-        <v>130</v>
+        <v>278</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>23</v>
       </c>
       <c r="G4" s="3">
-        <v>1920</v>
+        <v>1024</v>
       </c>
       <c r="H4" s="3">
-        <v>1200</v>
+        <v>768</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -687,10 +687,10 @@
         <v>20</v>
       </c>
       <c r="C5" s="3">
-        <v>441</v>
+        <v>57</v>
       </c>
       <c r="D5" s="3">
-        <v>130</v>
+        <v>278</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>24</v>
@@ -699,7 +699,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="3">
-        <v>1200</v>
+        <v>768</v>
       </c>
     </row>
     <row r="8" spans="1:17" s="1" customFormat="1">
@@ -746,11 +746,11 @@
       </c>
       <c r="C9" s="4">
         <f>C2</f>
-        <v>417</v>
+        <v>57</v>
       </c>
       <c r="D9" s="3">
         <f>D2</f>
-        <v>39</v>
+        <v>211</v>
       </c>
       <c r="E9" s="3">
         <v>1</v>
@@ -801,11 +801,11 @@
       </c>
       <c r="F10" s="7">
         <f>C2</f>
-        <v>417</v>
+        <v>57</v>
       </c>
       <c r="G10" s="7">
         <f>D2</f>
-        <v>39</v>
+        <v>211</v>
       </c>
       <c r="H10" s="7">
         <v>1</v>
@@ -856,11 +856,11 @@
       </c>
       <c r="I11" s="7">
         <f>C2</f>
-        <v>417</v>
+        <v>57</v>
       </c>
       <c r="J11" s="7">
         <f>D2</f>
-        <v>39</v>
+        <v>211</v>
       </c>
       <c r="K11" s="7">
         <v>1</v>
@@ -884,11 +884,11 @@
       </c>
       <c r="C12" s="4">
         <f>C3</f>
-        <v>861</v>
+        <v>231</v>
       </c>
       <c r="D12" s="7">
         <f>D3</f>
-        <v>39</v>
+        <v>211</v>
       </c>
       <c r="E12" s="7">
         <v>1</v>
@@ -916,7 +916,7 @@
       </c>
       <c r="M12" s="3">
         <f>-G3</f>
-        <v>-1920</v>
+        <v>-1024</v>
       </c>
       <c r="N12" s="5">
         <v>0</v>
@@ -940,11 +940,11 @@
       </c>
       <c r="F13" s="7">
         <f>C3</f>
-        <v>861</v>
+        <v>231</v>
       </c>
       <c r="G13" s="7">
         <f>D3</f>
-        <v>39</v>
+        <v>211</v>
       </c>
       <c r="H13" s="7">
         <v>1</v>
@@ -995,11 +995,11 @@
       </c>
       <c r="I14" s="7">
         <f>C3</f>
-        <v>861</v>
+        <v>231</v>
       </c>
       <c r="J14" s="7">
         <f>D3</f>
-        <v>39</v>
+        <v>211</v>
       </c>
       <c r="K14" s="7">
         <v>1</v>
@@ -1026,11 +1026,11 @@
       </c>
       <c r="C15" s="4">
         <f>C4</f>
-        <v>771</v>
+        <v>231</v>
       </c>
       <c r="D15" s="7">
         <f>D4</f>
-        <v>130</v>
+        <v>278</v>
       </c>
       <c r="E15" s="7">
         <v>1</v>
@@ -1061,7 +1061,7 @@
       </c>
       <c r="N15" s="5">
         <f>-G4</f>
-        <v>-1920</v>
+        <v>-1024</v>
       </c>
       <c r="P15" s="3" t="s">
         <v>13</v>
@@ -1085,11 +1085,11 @@
       </c>
       <c r="F16" s="7">
         <f>C4</f>
-        <v>771</v>
+        <v>231</v>
       </c>
       <c r="G16" s="7">
         <f>D4</f>
-        <v>130</v>
+        <v>278</v>
       </c>
       <c r="H16" s="7">
         <v>1</v>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="N16" s="5">
         <f>-H4</f>
-        <v>-1200</v>
+        <v>-768</v>
       </c>
       <c r="Q16" s="6">
         <v>0</v>
@@ -1141,11 +1141,11 @@
       </c>
       <c r="I17" s="7">
         <f>C4</f>
-        <v>771</v>
+        <v>231</v>
       </c>
       <c r="J17" s="7">
         <f>D4</f>
-        <v>130</v>
+        <v>278</v>
       </c>
       <c r="K17" s="7">
         <v>1</v>
@@ -1169,11 +1169,11 @@
       </c>
       <c r="C18" s="4">
         <f>C5</f>
-        <v>441</v>
+        <v>57</v>
       </c>
       <c r="D18" s="7">
         <f>D5</f>
-        <v>130</v>
+        <v>278</v>
       </c>
       <c r="E18" s="7">
         <v>1</v>
@@ -1224,11 +1224,11 @@
       </c>
       <c r="F19" s="7">
         <f>C5</f>
-        <v>441</v>
+        <v>57</v>
       </c>
       <c r="G19" s="7">
         <f>D5</f>
-        <v>130</v>
+        <v>278</v>
       </c>
       <c r="H19" s="7">
         <v>1</v>
@@ -1253,7 +1253,7 @@
       </c>
       <c r="Q19" s="6">
         <f>H5</f>
-        <v>1200</v>
+        <v>768</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -1280,11 +1280,11 @@
       </c>
       <c r="I20" s="7">
         <f>C5</f>
-        <v>441</v>
+        <v>57</v>
       </c>
       <c r="J20" s="7">
         <f>D5</f>
-        <v>130</v>
+        <v>278</v>
       </c>
       <c r="K20" s="7">
         <v>1</v>
@@ -1328,10 +1328,10 @@
       </c>
       <c r="C24" s="4">
         <f t="array" ref="C24:N35">MINVERSE(C9:N20)</f>
-        <v>2.5789152720677272E-19</v>
+        <v>9.6123205595251648E-19</v>
       </c>
       <c r="D24" s="7">
-        <v>-3.6036036036036041E-3</v>
+        <v>-7.6628352490421469E-3</v>
       </c>
       <c r="E24" s="7">
         <v>0</v>
@@ -1340,32 +1340,32 @@
         <v>0</v>
       </c>
       <c r="G24" s="7">
-        <v>3.6036036036036041E-3</v>
+        <v>7.6628352490421461E-3</v>
       </c>
       <c r="H24" s="7">
         <v>0</v>
       </c>
       <c r="I24" s="7">
-        <v>3.0303030303030307E-3</v>
+        <v>5.74712643678161E-3</v>
       </c>
       <c r="J24" s="7">
-        <v>-4.8484848484848502E-3</v>
+        <v>-7.6628352490421461E-3</v>
       </c>
       <c r="K24" s="7">
         <v>0</v>
       </c>
       <c r="L24" s="7">
-        <v>-3.0303030303030307E-3</v>
+        <v>-5.74712643678161E-3</v>
       </c>
       <c r="M24" s="7">
-        <v>4.8484848484848502E-3</v>
+        <v>7.6628352490421469E-3</v>
       </c>
       <c r="N24" s="5">
         <v>0</v>
       </c>
       <c r="Q24" s="6">
         <f t="array" ref="Q24:Q35">MMULT(C24:N35, Q9:Q20)</f>
-        <v>5.8181818181818201</v>
+        <v>5.8850574712643686</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -1373,10 +1373,10 @@
         <v>2</v>
       </c>
       <c r="C25" s="4">
-        <v>-1.0989010989010988E-2</v>
+        <v>-1.4925373134328361E-2</v>
       </c>
       <c r="D25" s="7">
-        <v>9.5040095040095044E-4</v>
+        <v>4.9139031382501038E-19</v>
       </c>
       <c r="E25" s="7">
         <v>0</v>
@@ -1385,31 +1385,31 @@
         <v>0</v>
       </c>
       <c r="G25" s="7">
-        <v>-9.5040095040095044E-4</v>
+        <v>-2.4569515691250519E-19</v>
       </c>
       <c r="H25" s="7">
         <v>0</v>
       </c>
       <c r="I25" s="7">
-        <v>-7.992007992007992E-4</v>
+        <v>6.1423789228126296E-19</v>
       </c>
       <c r="J25" s="7">
-        <v>1.2787212787212805E-3</v>
+        <v>2.4569515691250519E-19</v>
       </c>
       <c r="K25" s="7">
         <v>0</v>
       </c>
       <c r="L25" s="7">
-        <v>1.1788211788211787E-2</v>
+        <v>1.492537313432836E-2</v>
       </c>
       <c r="M25" s="7">
-        <v>-1.2787212787212805E-3</v>
+        <v>-4.9139031382501038E-19</v>
       </c>
       <c r="N25" s="5">
         <v>0</v>
       </c>
       <c r="Q25" s="6">
-        <v>-1.5344655344655365</v>
+        <v>-3.77387761017608E-16</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -1417,10 +1417,10 @@
         <v>3</v>
       </c>
       <c r="C26" s="4">
-        <v>1.4285714285714284</v>
+        <v>4.1492537313432845</v>
       </c>
       <c r="D26" s="7">
-        <v>1.4656370656370659</v>
+        <v>0.43678160919540221</v>
       </c>
       <c r="E26" s="7">
         <v>0</v>
@@ -1429,31 +1429,31 @@
         <v>0</v>
       </c>
       <c r="G26" s="7">
-        <v>-1.4656370656370659</v>
+        <v>-0.43678160919540221</v>
       </c>
       <c r="H26" s="7">
         <v>0</v>
       </c>
       <c r="I26" s="7">
-        <v>-1.2324675324675327</v>
+        <v>-0.32758620689655188</v>
       </c>
       <c r="J26" s="7">
-        <v>1.9719480519480523</v>
+        <v>0.43678160919540221</v>
       </c>
       <c r="K26" s="7">
         <v>0</v>
       </c>
       <c r="L26" s="7">
-        <v>0.803896103896104</v>
+        <v>-2.8216675244467324</v>
       </c>
       <c r="M26" s="7">
-        <v>-1.9719480519480523</v>
+        <v>-0.43678160919540221</v>
       </c>
       <c r="N26" s="5">
         <v>0</v>
       </c>
       <c r="Q26" s="6">
-        <v>-2366.337662337663</v>
+        <v>-335.4482758620689</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -1464,7 +1464,7 @@
         <v>0</v>
       </c>
       <c r="D27" s="7">
-        <v>-2.2522522522522527E-3</v>
+        <v>-5.7471264367816082E-3</v>
       </c>
       <c r="E27" s="7">
         <v>0</v>
@@ -1473,7 +1473,7 @@
         <v>0</v>
       </c>
       <c r="G27" s="7">
-        <v>2.2522522522522522E-3</v>
+        <v>5.74712643678161E-3</v>
       </c>
       <c r="H27" s="7">
         <v>0</v>
@@ -1508,7 +1508,7 @@
         <v>0</v>
       </c>
       <c r="D28" s="7">
-        <v>-1.0395010395010394E-2</v>
+        <v>-1.4925373134328361E-2</v>
       </c>
       <c r="E28" s="7">
         <v>0</v>
@@ -1517,7 +1517,7 @@
         <v>0</v>
       </c>
       <c r="G28" s="7">
-        <v>-5.9400059400059417E-4</v>
+        <v>6.1423789228126296E-19</v>
       </c>
       <c r="H28" s="7">
         <v>0</v>
@@ -1535,13 +1535,13 @@
         <v>0</v>
       </c>
       <c r="M28" s="7">
-        <v>1.0989010989010988E-2</v>
+        <v>1.4925373134328361E-2</v>
       </c>
       <c r="N28" s="5">
         <v>0</v>
       </c>
       <c r="Q28" s="6">
-        <v>13.186813186813186</v>
+        <v>11.462686567164182</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -1552,7 +1552,7 @@
         <v>0</v>
       </c>
       <c r="D29" s="7">
-        <v>2.3445945945945947</v>
+        <v>4.4768399382398361</v>
       </c>
       <c r="E29" s="7">
         <v>0</v>
@@ -1561,7 +1561,7 @@
         <v>0</v>
       </c>
       <c r="G29" s="7">
-        <v>-0.91602316602316602</v>
+        <v>-0.32758620689655188</v>
       </c>
       <c r="H29" s="7">
         <v>0</v>
@@ -1579,13 +1579,13 @@
         <v>0</v>
       </c>
       <c r="M29" s="7">
-        <v>-0.42857142857142855</v>
+        <v>-3.1492537313432845</v>
       </c>
       <c r="N29" s="5">
         <v>0</v>
       </c>
       <c r="Q29" s="6">
-        <v>-514.28571428571422</v>
+        <v>-2418.6268656716425</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -1596,10 +1596,10 @@
         <v>14</v>
       </c>
       <c r="C30" s="4">
-        <v>0</v>
+        <v>9.3870317964112938E-22</v>
       </c>
       <c r="D30" s="7">
-        <v>-1.8768768768768768E-6</v>
+        <v>-7.4832375478927216E-6</v>
       </c>
       <c r="E30" s="7">
         <v>0</v>
@@ -1608,34 +1608,34 @@
         <v>0</v>
       </c>
       <c r="G30" s="7">
-        <v>1.8768768768768768E-6</v>
+        <v>7.4832375478927208E-6</v>
       </c>
       <c r="H30" s="7">
-        <v>2.5789152720677272E-19</v>
+        <v>0</v>
       </c>
       <c r="I30" s="7">
-        <v>-1.2592359726893199E-22</v>
+        <v>0</v>
       </c>
       <c r="J30" s="7">
-        <v>-2.5252525252525262E-6</v>
+        <v>-7.4832375478927208E-6</v>
       </c>
       <c r="K30" s="7">
-        <v>3.0303030303030307E-3</v>
+        <v>5.7471264367816082E-3</v>
       </c>
       <c r="L30" s="7">
-        <v>1.2592359726893199E-22</v>
+        <v>-9.3870317964112938E-22</v>
       </c>
       <c r="M30" s="7">
-        <v>2.5252525252525262E-6</v>
+        <v>7.4832375478927216E-6</v>
       </c>
       <c r="N30" s="5">
-        <v>-3.0303030303030303E-3</v>
+        <v>-5.7471264367816082E-3</v>
       </c>
       <c r="P30" s="3" t="s">
         <v>15</v>
       </c>
       <c r="Q30" s="6">
-        <v>1.3010426069826053E-18</v>
+        <v>1.7347234759768071E-18</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -1643,43 +1643,43 @@
         <v>8</v>
       </c>
       <c r="C31" s="4">
-        <v>-5.7234432234432226E-6</v>
+        <v>-1.457555970149254E-5</v>
       </c>
       <c r="D31" s="7">
-        <v>4.950004950004949E-7</v>
+        <v>4.798733533447367E-22</v>
       </c>
       <c r="E31" s="7">
         <v>0</v>
       </c>
       <c r="F31" s="7">
-        <v>5.7234432234432226E-6</v>
+        <v>1.4575559701492537E-5</v>
       </c>
       <c r="G31" s="7">
-        <v>-4.950004950004949E-7</v>
+        <v>-2.3993667667236835E-22</v>
       </c>
       <c r="H31" s="7">
-        <v>-1.0989010989010988E-2</v>
+        <v>-1.4925373134328358E-2</v>
       </c>
       <c r="I31" s="7">
-        <v>-7.7006327006327023E-6</v>
+        <v>-1.4575559701492537E-5</v>
       </c>
       <c r="J31" s="7">
-        <v>6.6600066600066676E-7</v>
+        <v>2.3993667667236835E-22</v>
       </c>
       <c r="K31" s="7">
-        <v>1.3986013986013986E-2</v>
+        <v>1.4925373134328358E-2</v>
       </c>
       <c r="L31" s="7">
-        <v>7.7006327006327023E-6</v>
+        <v>1.457555970149254E-5</v>
       </c>
       <c r="M31" s="7">
-        <v>-6.6600066600066676E-7</v>
+        <v>-4.798733533447367E-22</v>
       </c>
       <c r="N31" s="5">
-        <v>-2.9970029970029966E-3</v>
+        <v>0</v>
       </c>
       <c r="Q31" s="6">
-        <v>-3.7962037962037966E-3</v>
+        <v>-3.6854273536875781E-19</v>
       </c>
     </row>
     <row r="32" spans="1:17">
@@ -1687,43 +1687,43 @@
         <v>9</v>
       </c>
       <c r="C32" s="4">
-        <v>7.4404761904761901E-4</v>
+        <v>4.0520055970149262E-3</v>
       </c>
       <c r="D32" s="7">
-        <v>7.6335263835263835E-4</v>
+        <v>4.2654454022988497E-4</v>
       </c>
       <c r="E32" s="7">
         <v>0</v>
       </c>
       <c r="F32" s="7">
-        <v>-7.4404761904761901E-4</v>
+        <v>-4.0520055970149254E-3</v>
       </c>
       <c r="G32" s="7">
-        <v>-7.6335263835263835E-4</v>
+        <v>-4.2654454022988497E-4</v>
       </c>
       <c r="H32" s="7">
-        <v>1.4285714285714284</v>
+        <v>4.1492537313432836</v>
       </c>
       <c r="I32" s="7">
-        <v>1.0010822510822513E-3</v>
+        <v>4.0520055970149254E-3</v>
       </c>
       <c r="J32" s="7">
-        <v>1.0270562770562772E-3</v>
+        <v>4.2654454022988497E-4</v>
       </c>
       <c r="K32" s="7">
-        <v>-3.1545454545454548</v>
+        <v>-4.4768399382398352</v>
       </c>
       <c r="L32" s="7">
-        <v>-1.0010822510822513E-3</v>
+        <v>-4.0520055970149262E-3</v>
       </c>
       <c r="M32" s="7">
-        <v>-1.0270562770562772E-3</v>
+        <v>-4.2654454022988497E-4</v>
       </c>
       <c r="N32" s="5">
-        <v>2.7259740259740259</v>
+        <v>1.3275862068965516</v>
       </c>
       <c r="Q32" s="6">
-        <v>1.4935064935064934</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:17">
@@ -1731,7 +1731,7 @@
         <v>10</v>
       </c>
       <c r="C33" s="4">
-        <v>5.2083333333333333E-4</v>
+        <v>9.765625E-4</v>
       </c>
       <c r="D33" s="7">
         <v>0</v>
@@ -1740,34 +1740,34 @@
         <v>-1</v>
       </c>
       <c r="F33" s="7">
-        <v>-5.2083333333333333E-4</v>
+        <v>-9.7656249999999978E-4</v>
       </c>
       <c r="G33" s="7">
         <v>0</v>
       </c>
       <c r="H33" s="7">
-        <v>1</v>
+        <v>0.99999999999999978</v>
       </c>
       <c r="I33" s="7">
-        <v>7.0075757575757582E-4</v>
+        <v>9.7656249999999978E-4</v>
       </c>
       <c r="J33" s="7">
         <v>0</v>
       </c>
       <c r="K33" s="7">
-        <v>-1.3454545454545455</v>
+        <v>-0.99999999999999978</v>
       </c>
       <c r="L33" s="7">
-        <v>-7.0075757575757582E-4</v>
+        <v>-9.765625E-4</v>
       </c>
       <c r="M33" s="7">
         <v>0</v>
       </c>
       <c r="N33" s="5">
-        <v>1.3454545454545455</v>
+        <v>1</v>
       </c>
       <c r="Q33" s="6">
-        <v>1.3454545454545455</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:17">
@@ -1775,43 +1775,43 @@
         <v>11</v>
       </c>
       <c r="C34" s="4">
-        <v>5.2083333333333333E-4</v>
+        <v>9.7656250000000022E-4</v>
       </c>
       <c r="D34" s="7">
-        <v>-8.3333333333333328E-4</v>
+        <v>-1.3020833333333337E-3</v>
       </c>
       <c r="E34" s="7">
         <v>0</v>
       </c>
       <c r="F34" s="7">
-        <v>-5.2083333333333333E-4</v>
+        <v>-9.765625E-4</v>
       </c>
       <c r="G34" s="7">
-        <v>8.3333333333333328E-4</v>
+        <v>1.3020833333333335E-3</v>
       </c>
       <c r="H34" s="7">
         <v>0</v>
       </c>
       <c r="I34" s="7">
-        <v>7.0075757575757582E-4</v>
+        <v>9.765625E-4</v>
       </c>
       <c r="J34" s="7">
-        <v>-1.1212121212121214E-3</v>
+        <v>-1.3020833333333335E-3</v>
       </c>
       <c r="K34" s="7">
         <v>0</v>
       </c>
       <c r="L34" s="7">
-        <v>-7.0075757575757582E-4</v>
+        <v>-9.7656250000000022E-4</v>
       </c>
       <c r="M34" s="7">
-        <v>1.1212121212121214E-3</v>
+        <v>1.3020833333333337E-3</v>
       </c>
       <c r="N34" s="5">
         <v>0</v>
       </c>
       <c r="Q34" s="6">
-        <v>1.3454545454545457</v>
+        <v>1.0000000000000002</v>
       </c>
     </row>
     <row r="35" spans="1:17">
@@ -1822,7 +1822,7 @@
         <v>0</v>
       </c>
       <c r="D35" s="7">
-        <v>-6.1936936936936933E-4</v>
+        <v>-1.3020833333333337E-3</v>
       </c>
       <c r="E35" s="7">
         <v>0</v>
@@ -1831,7 +1831,7 @@
         <v>0</v>
       </c>
       <c r="G35" s="7">
-        <v>6.1936936936936933E-4</v>
+        <v>1.3020833333333335E-3</v>
       </c>
       <c r="H35" s="7">
         <v>0</v>
@@ -1840,7 +1840,7 @@
         <v>0</v>
       </c>
       <c r="J35" s="7">
-        <v>-8.3333333333333339E-4</v>
+        <v>-1.3020833333333335E-3</v>
       </c>
       <c r="K35" s="7">
         <v>0</v>
@@ -1849,13 +1849,13 @@
         <v>0</v>
       </c>
       <c r="M35" s="7">
-        <v>8.3333333333333339E-4</v>
+        <v>1.3020833333333337E-3</v>
       </c>
       <c r="N35" s="5">
         <v>0</v>
       </c>
       <c r="Q35" s="6">
-        <v>1</v>
+        <v>1.0000000000000002</v>
       </c>
     </row>
     <row r="40" spans="1:17">
@@ -1867,7 +1867,7 @@
       </c>
       <c r="E40" s="3">
         <f>Q24</f>
-        <v>5.8181818181818201</v>
+        <v>5.8850574712643686</v>
       </c>
     </row>
     <row r="41" spans="1:17">
@@ -1876,7 +1876,7 @@
       </c>
       <c r="E41" s="3">
         <f t="shared" ref="E41:E51" si="0">Q25</f>
-        <v>-1.5344655344655365</v>
+        <v>-3.77387761017608E-16</v>
       </c>
     </row>
     <row r="42" spans="1:17">
@@ -1885,7 +1885,7 @@
       </c>
       <c r="E42" s="3">
         <f t="shared" si="0"/>
-        <v>-2366.337662337663</v>
+        <v>-335.4482758620689</v>
       </c>
     </row>
     <row r="43" spans="1:17">
@@ -1898,15 +1898,15 @@
       </c>
       <c r="J43" s="9">
         <f>E40</f>
-        <v>5.8181818181818201</v>
+        <v>5.8850574712643686</v>
       </c>
       <c r="K43" s="10">
         <f>E41</f>
-        <v>-1.5344655344655365</v>
+        <v>-3.77387761017608E-16</v>
       </c>
       <c r="L43" s="11">
         <f>E42</f>
-        <v>-2366.337662337663</v>
+        <v>-335.4482758620689</v>
       </c>
     </row>
     <row r="44" spans="1:17">
@@ -1915,7 +1915,7 @@
       </c>
       <c r="E44" s="3">
         <f t="shared" si="0"/>
-        <v>13.186813186813186</v>
+        <v>11.462686567164182</v>
       </c>
       <c r="I44" s="3" t="s">
         <v>25</v>
@@ -1926,11 +1926,11 @@
       </c>
       <c r="K44" s="10">
         <f>E44</f>
-        <v>13.186813186813186</v>
+        <v>11.462686567164182</v>
       </c>
       <c r="L44" s="11">
         <f>E45</f>
-        <v>-514.28571428571422</v>
+        <v>-2418.6268656716425</v>
       </c>
     </row>
     <row r="45" spans="1:17">
@@ -1939,19 +1939,19 @@
       </c>
       <c r="E45" s="3">
         <f t="shared" si="0"/>
-        <v>-514.28571428571422</v>
+        <v>-2418.6268656716425</v>
       </c>
       <c r="J45" s="9">
         <f>E46</f>
-        <v>1.3010426069826053E-18</v>
+        <v>1.7347234759768071E-18</v>
       </c>
       <c r="K45" s="10">
         <f>E47</f>
-        <v>-3.7962037962037966E-3</v>
+        <v>-3.6854273536875781E-19</v>
       </c>
       <c r="L45" s="11">
         <f>E48</f>
-        <v>1.4935064935064934</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:17">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="E46" s="3">
         <f t="shared" si="0"/>
-        <v>1.3010426069826053E-18</v>
+        <v>1.7347234759768071E-18</v>
       </c>
     </row>
     <row r="47" spans="1:17">
@@ -1969,7 +1969,7 @@
       </c>
       <c r="E47" s="3">
         <f t="shared" si="0"/>
-        <v>-3.7962037962037966E-3</v>
+        <v>-3.6854273536875781E-19</v>
       </c>
     </row>
     <row r="48" spans="1:17">
@@ -1978,14 +1978,14 @@
       </c>
       <c r="E48" s="3">
         <f t="shared" si="0"/>
-        <v>1.4935064935064934</v>
+        <v>1</v>
       </c>
       <c r="I48" s="3" t="s">
         <v>26</v>
       </c>
       <c r="J48" s="6">
         <f>E49</f>
-        <v>1.3454545454545455</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="4:10">
@@ -1994,11 +1994,11 @@
       </c>
       <c r="E49" s="3">
         <f t="shared" si="0"/>
-        <v>1.3454545454545455</v>
+        <v>1</v>
       </c>
       <c r="J49" s="6">
         <f>E50</f>
-        <v>1.3454545454545457</v>
+        <v>1.0000000000000002</v>
       </c>
     </row>
     <row r="50" spans="4:10">
@@ -2007,11 +2007,11 @@
       </c>
       <c r="E50" s="3">
         <f t="shared" si="0"/>
-        <v>1.3454545454545457</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="J50" s="6">
         <f>E51</f>
-        <v>1</v>
+        <v>1.0000000000000002</v>
       </c>
     </row>
     <row r="51" spans="4:10">
@@ -2020,7 +2020,7 @@
       </c>
       <c r="E51" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="J51" s="6">
         <f>E52</f>

</xml_diff>